<commit_message>
remove nav bar from home + remove background from show pages
</commit_message>
<xml_diff>
--- a/markdown + erd + wireframes + spreadsheet/neat-150730.xlsx
+++ b/markdown + erd + wireframes + spreadsheet/neat-150730.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="520" windowWidth="23920" windowHeight="14900" tabRatio="936"/>
+    <workbookView xWindow="300" yWindow="520" windowWidth="23920" windowHeight="14900" tabRatio="936"/>
   </bookViews>
   <sheets>
     <sheet name="neat-todo" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3556" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3567" uniqueCount="606">
   <si>
     <t>Date</t>
   </si>
@@ -1757,9 +1757,6 @@
     <t>if I change any of the data in seeds</t>
   </si>
   <si>
-    <t>Finally, I will be able to enter new whiskeys after an event.</t>
-  </si>
-  <si>
     <t>need to change database from sqllite to postgres</t>
   </si>
   <si>
@@ -1769,36 +1766,12 @@
     <t>NAV BAR</t>
   </si>
   <si>
-    <t>inline, not block</t>
-  </si>
-  <si>
-    <t>remove underline</t>
-  </si>
-  <si>
-    <t>remove bullets</t>
-  </si>
-  <si>
-    <t>fix colors- yellow</t>
-  </si>
-  <si>
     <t>SHOW WHISKEY PAGE</t>
   </si>
   <si>
-    <t>RULES PAGE</t>
-  </si>
-  <si>
-    <t>ADD COMMENT TO SHOW PAGE</t>
-  </si>
-  <si>
     <t>image on left, data on right</t>
   </si>
   <si>
-    <t>have on every page!!!</t>
-  </si>
-  <si>
-    <t>only if I have time</t>
-  </si>
-  <si>
     <t>link as many images as possible</t>
   </si>
   <si>
@@ -1808,31 +1781,76 @@
     <t>LOGIN PAGE</t>
   </si>
   <si>
-    <t>link page to home, sessions, etc.</t>
-  </si>
-  <si>
     <t>TWEAK NEW WHISKEY FORM</t>
   </si>
   <si>
     <t>GA STUFF</t>
   </si>
   <si>
-    <t>look table headers to page?</t>
-  </si>
-  <si>
-    <t>have all columns sortable</t>
-  </si>
-  <si>
-    <t>where do I put it?</t>
-  </si>
-  <si>
-    <t>hour</t>
-  </si>
-  <si>
-    <t>hours</t>
-  </si>
-  <si>
-    <t>Controllers singular and plural!!!!</t>
+    <t>git checkout nav</t>
+  </si>
+  <si>
+    <t>git branch nav</t>
+  </si>
+  <si>
+    <t>git branch</t>
+  </si>
+  <si>
+    <t>home page image showing on ALL show pages</t>
+  </si>
+  <si>
+    <t>doesn't seem to be working?</t>
+  </si>
+  <si>
+    <t>enter new whiskeys after an event.</t>
+  </si>
+  <si>
+    <t>CREATE NEW MEMBER FORM</t>
+  </si>
+  <si>
+    <t>enter/ delete new members after an event.</t>
+  </si>
+  <si>
+    <t>how to make so only member id 1 or 2 can edit</t>
+  </si>
+  <si>
+    <t>shows which branch we are on and what is available</t>
+  </si>
+  <si>
+    <t>switches to the nav branch</t>
+  </si>
+  <si>
+    <t>ADD NEW COMMENT TO SHOW PAGE</t>
+  </si>
+  <si>
+    <t>does this have to do with where css files are stored? Should I use application.css?</t>
+  </si>
+  <si>
+    <t>remove underline on logo, change color to dark yellow</t>
+  </si>
+  <si>
+    <t>fix colors- dark yellow #F1C232</t>
+  </si>
+  <si>
+    <t>remove nav bar from home page - can I use:</t>
+  </si>
+  <si>
+    <t>background:transparent;</t>
+  </si>
+  <si>
+    <t>border: 0px;</t>
+  </si>
+  <si>
+    <t>display all whiskey's comments on whiskey show page</t>
+  </si>
+  <si>
+    <t>WHISKEY IMAGES</t>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/540/brbon_rid1.jpg</t>
+  </si>
+  <si>
+    <t>https://img.thewhiskyexchange.com/900/ablob.non27.jpg</t>
   </si>
 </sst>
 </file>
@@ -1966,7 +1984,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="387">
+  <cellStyleXfs count="411">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2354,6 +2372,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2518,7 +2560,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="387">
+  <cellStyles count="411">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -2741,6 +2783,18 @@
     <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="385" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2905,6 +2959,18 @@
     <cellStyle name="Hyperlink" xfId="324" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="326" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="328" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3420,186 +3486,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D34"/>
+  <dimension ref="A2:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="62.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.1640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
-      <c r="B2" t="s">
-        <v>599</v>
-      </c>
-      <c r="C2" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    <row r="2" spans="1:6">
+      <c r="A2" s="21"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="21"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="21"/>
-      <c r="B4" s="22" t="s">
+      <c r="B3" s="22" t="s">
+        <v>583</v>
+      </c>
+      <c r="E3" t="s">
+        <v>586</v>
+      </c>
+      <c r="F3" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>574</v>
+      </c>
+      <c r="E4" t="s">
+        <v>585</v>
+      </c>
+      <c r="F4" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="B5" t="s">
         <v>575</v>
       </c>
-      <c r="C5" s="21">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:6">
+      <c r="E6" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="22" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="B6" t="s">
-        <v>576</v>
-      </c>
-      <c r="C6" s="21">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" s="22" t="s">
+    <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="22" t="s">
         <v>577</v>
       </c>
-      <c r="C9" s="21">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="B10" t="s">
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="B11" t="s">
+    <row r="20" spans="2:6">
+      <c r="B20" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="22" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="22" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" t="s">
+        <v>588</v>
+      </c>
+      <c r="E27" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="E28" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="E29" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30" s="22" t="s">
+        <v>582</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" t="s">
+        <v>589</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="E32" s="29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="E33" s="29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="22" t="s">
+        <v>590</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" t="s">
+        <v>591</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="B36" t="s">
+        <v>592</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="E37" s="29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="B40" s="22" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="B41" t="s">
         <v>579</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="B12" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="B13" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="B14" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="B15" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="B16" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="22" t="s">
-        <v>582</v>
-      </c>
-      <c r="C18" s="21">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="22" t="s">
-        <v>584</v>
-      </c>
-      <c r="C22" s="21">
-        <v>2</v>
-      </c>
-      <c r="D22" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25" s="22" t="s">
-        <v>590</v>
-      </c>
-      <c r="C25" s="21">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="22" t="s">
-        <v>592</v>
-      </c>
-      <c r="C29" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="D29" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="22" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" t="s">
-        <v>587</v>
       </c>
     </row>
   </sheetData>
@@ -3868,7 +3961,7 @@
         <v>386</v>
       </c>
       <c r="W4" s="28">
-        <f>COUNTIF(E4:V4,"T")</f>
+        <f t="shared" ref="W4:W23" si="0">COUNTIF(E4:V4,"T")</f>
         <v>18</v>
       </c>
     </row>
@@ -3922,7 +4015,7 @@
         <v>386</v>
       </c>
       <c r="W5" s="28">
-        <f>COUNTIF(E5:V5,"T")</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
@@ -3970,7 +4063,7 @@
         <v>386</v>
       </c>
       <c r="W6" s="28">
-        <f>COUNTIF(E6:V6,"T")</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
@@ -4012,7 +4105,7 @@
         <v>386</v>
       </c>
       <c r="W7" s="28">
-        <f>COUNTIF(E7:V7,"T")</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -4045,7 +4138,7 @@
         <v>386</v>
       </c>
       <c r="W8" s="28">
-        <f>COUNTIF(E8:V8,"T")</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -4093,7 +4186,7 @@
         <v>386</v>
       </c>
       <c r="W9" s="28">
-        <f>COUNTIF(E9:V9,"T")</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
@@ -4130,7 +4223,7 @@
         <v>386</v>
       </c>
       <c r="W10" s="28">
-        <f>COUNTIF(E10:V10,"T")</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -4154,7 +4247,7 @@
         <v>386</v>
       </c>
       <c r="W11" s="28">
-        <f>COUNTIF(E11:V11,"T")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -4199,7 +4292,7 @@
         <v>386</v>
       </c>
       <c r="W12" s="28">
-        <f>COUNTIF(E12:V12,"T")</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -4220,7 +4313,7 @@
         <v>386</v>
       </c>
       <c r="W13" s="28">
-        <f>COUNTIF(E13:V13,"T")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -4238,7 +4331,7 @@
         <v>386</v>
       </c>
       <c r="W14" s="28">
-        <f>COUNTIF(E14:V14,"T")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4256,7 +4349,7 @@
         <v>386</v>
       </c>
       <c r="W15" s="28">
-        <f>COUNTIF(E15:V15,"T")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4283,7 +4376,7 @@
         <v>386</v>
       </c>
       <c r="W16" s="28">
-        <f>COUNTIF(E16:V16,"T")</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -4301,7 +4394,7 @@
         <v>386</v>
       </c>
       <c r="W17" s="28">
-        <f>COUNTIF(E17:V17,"T")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4319,7 +4412,7 @@
         <v>386</v>
       </c>
       <c r="W18" s="28">
-        <f>COUNTIF(E18:V18,"T")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4337,7 +4430,7 @@
         <v>386</v>
       </c>
       <c r="W19" s="28">
-        <f>COUNTIF(E19:V19,"T")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4356,7 +4449,7 @@
         <v>386</v>
       </c>
       <c r="W20" s="28">
-        <f>COUNTIF(E20:V20,"T")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4377,7 +4470,7 @@
         <v>386</v>
       </c>
       <c r="W21" s="28">
-        <f>COUNTIF(E21:V21,"T")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -4395,7 +4488,7 @@
         <v>386</v>
       </c>
       <c r="W22" s="28">
-        <f>COUNTIF(E22:V22,"T")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4413,7 +4506,7 @@
         <v>386</v>
       </c>
       <c r="W23" s="28">
-        <f>COUNTIF(E23:V23,"T")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4422,71 +4515,71 @@
     </row>
     <row r="25" spans="1:23">
       <c r="E25" s="28">
-        <f t="shared" ref="E25:U25" si="0">COUNTIF(E3:E22,"T")</f>
+        <f t="shared" ref="E25:U25" si="1">COUNTIF(E3:E22,"T")</f>
         <v>8</v>
       </c>
       <c r="F25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="H25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="J25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="K25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="L25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="M25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="N25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="O25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="P25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="Q25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="R25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="S25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="T25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="U25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="V25" s="28">
@@ -8682,9 +8775,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB118"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z2" sqref="Z2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17919,7 +18012,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
add new comment in show + logo color yellow
</commit_message>
<xml_diff>
--- a/markdown + erd + wireframes + spreadsheet/neat-150730.xlsx
+++ b/markdown + erd + wireframes + spreadsheet/neat-150730.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="520" windowWidth="23920" windowHeight="14900" tabRatio="936" activeTab="3"/>
+    <workbookView xWindow="320" yWindow="520" windowWidth="23920" windowHeight="14900" tabRatio="936"/>
   </bookViews>
   <sheets>
     <sheet name="neat-todo" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3857" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3634" uniqueCount="685">
   <si>
     <t>Date</t>
   </si>
@@ -1763,9 +1763,6 @@
     <t>SHOW WHISKEY PAGE</t>
   </si>
   <si>
-    <t>image on left, data on right</t>
-  </si>
-  <si>
     <t>link as many images as possible</t>
   </si>
   <si>
@@ -2078,16 +2075,19 @@
     <t>https://img.thewhiskyexchange.com/540/mnmsig1991.jpg</t>
   </si>
   <si>
-    <t>Macallan 18</t>
-  </si>
-  <si>
-    <t>Macallan Cask Strength</t>
-  </si>
-  <si>
     <t>https://img.thewhiskyexchange.com/540/macob.18yo.jpg</t>
   </si>
   <si>
     <t>https://img.thewhiskyexchange.com/900/macob.10yov7.jpg</t>
+  </si>
+  <si>
+    <t>css fixed height</t>
+  </si>
+  <si>
+    <t>html heights</t>
+  </si>
+  <si>
+    <t>image resizing</t>
   </si>
 </sst>
 </file>
@@ -4657,9 +4657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F142"/>
   <sheetViews>
-    <sheetView topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26:F142"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -4678,29 +4676,29 @@
         <v>574</v>
       </c>
       <c r="E3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -4711,974 +4709,519 @@
         <v>575</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>576</v>
-      </c>
-    </row>
     <row r="11" spans="1:6">
       <c r="B11" t="s">
-        <v>589</v>
+        <v>588</v>
+      </c>
+      <c r="E11" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" s="22" t="s">
-        <v>588</v>
+        <v>587</v>
+      </c>
+      <c r="E12" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="E14" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="22" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="22" t="s">
+    <row r="18" spans="2:5">
+      <c r="B18" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
-      <c r="B18" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6">
-      <c r="E26" s="48" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6">
-      <c r="E27" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6">
-      <c r="E28" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6">
+    <row r="26" spans="2:5">
+      <c r="E26" s="48"/>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="E27" s="29"/>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="E28" s="29"/>
+    </row>
+    <row r="29" spans="2:5">
       <c r="B29" s="22" t="s">
-        <v>578</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>324</v>
-      </c>
-      <c r="F29" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6">
+        <v>577</v>
+      </c>
+      <c r="E29" s="29"/>
+    </row>
+    <row r="30" spans="2:5">
       <c r="B30" t="s">
-        <v>582</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6">
-      <c r="E31" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="F31" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6">
-      <c r="E32" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" t="s">
-        <v>597</v>
-      </c>
+        <v>581</v>
+      </c>
+      <c r="E30" s="29"/>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="E31" s="29"/>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="E32" s="29"/>
     </row>
     <row r="33" spans="2:6">
       <c r="B33" s="22" t="s">
-        <v>583</v>
-      </c>
-      <c r="E33" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F33" t="s">
-        <v>594</v>
-      </c>
+        <v>582</v>
+      </c>
+      <c r="E33" s="29"/>
     </row>
     <row r="34" spans="2:6">
       <c r="B34" t="s">
-        <v>584</v>
-      </c>
-      <c r="E34" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="F34" t="s">
-        <v>598</v>
-      </c>
+        <v>583</v>
+      </c>
+      <c r="E34" s="29"/>
     </row>
     <row r="35" spans="2:6">
       <c r="B35" t="s">
-        <v>585</v>
-      </c>
-      <c r="E35" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" t="s">
-        <v>599</v>
-      </c>
+        <v>584</v>
+      </c>
+      <c r="E35" s="29"/>
     </row>
     <row r="36" spans="2:6">
-      <c r="E36" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" t="s">
-        <v>600</v>
-      </c>
+      <c r="E36" s="29"/>
     </row>
     <row r="37" spans="2:6">
-      <c r="E37" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="F37" s="52" t="s">
-        <v>311</v>
-      </c>
+      <c r="E37" s="29"/>
+      <c r="F37" s="52"/>
     </row>
     <row r="38" spans="2:6">
       <c r="B38" s="22" t="s">
-        <v>590</v>
-      </c>
-      <c r="E38" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="F38" s="52" t="s">
-        <v>342</v>
-      </c>
+        <v>589</v>
+      </c>
+      <c r="E38" s="29"/>
+      <c r="F38" s="52"/>
     </row>
     <row r="39" spans="2:6">
       <c r="B39" t="s">
-        <v>577</v>
-      </c>
-      <c r="E39" s="29" t="s">
-        <v>325</v>
-      </c>
-      <c r="F39" s="52" t="s">
-        <v>602</v>
-      </c>
+        <v>576</v>
+      </c>
+      <c r="E39" s="29"/>
+      <c r="F39" s="52"/>
     </row>
     <row r="40" spans="2:6">
-      <c r="E40" s="29" t="s">
-        <v>343</v>
-      </c>
-      <c r="F40" s="52" t="s">
-        <v>404</v>
-      </c>
+      <c r="E40" s="29"/>
+      <c r="F40" s="52"/>
     </row>
     <row r="41" spans="2:6">
-      <c r="E41" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="F41" s="52" t="s">
-        <v>601</v>
-      </c>
+      <c r="E41" s="29"/>
+      <c r="F41" s="52"/>
     </row>
     <row r="42" spans="2:6">
-      <c r="E42" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="F42" s="52" t="s">
-        <v>603</v>
-      </c>
+      <c r="E42" s="29"/>
+      <c r="F42" s="52"/>
     </row>
     <row r="43" spans="2:6">
-      <c r="E43" s="29" t="s">
-        <v>344</v>
-      </c>
-      <c r="F43" s="52" t="s">
-        <v>406</v>
-      </c>
+      <c r="E43" s="29"/>
+      <c r="F43" s="52"/>
     </row>
     <row r="44" spans="2:6">
-      <c r="E44" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="F44" s="52" t="s">
-        <v>407</v>
-      </c>
+      <c r="E44" s="29"/>
+      <c r="F44" s="52"/>
     </row>
     <row r="45" spans="2:6">
-      <c r="E45" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="F45" s="54" t="s">
-        <v>604</v>
-      </c>
+      <c r="E45" s="48"/>
+      <c r="F45" s="54"/>
     </row>
     <row r="46" spans="2:6">
-      <c r="E46" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="F46" s="52" t="s">
-        <v>605</v>
-      </c>
+      <c r="E46" s="29"/>
+      <c r="F46" s="52"/>
     </row>
     <row r="47" spans="2:6">
-      <c r="E47" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="F47" s="52" t="s">
-        <v>606</v>
-      </c>
+      <c r="E47" s="29"/>
+      <c r="F47" s="52"/>
     </row>
     <row r="48" spans="2:6">
-      <c r="E48" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="F48" s="52" t="s">
-        <v>607</v>
-      </c>
+      <c r="E48" s="29"/>
+      <c r="F48" s="52"/>
     </row>
     <row r="49" spans="5:6">
-      <c r="E49" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="F49" s="34" t="s">
-        <v>408</v>
-      </c>
+      <c r="E49" s="29"/>
+      <c r="F49" s="34"/>
     </row>
     <row r="50" spans="5:6">
-      <c r="E50" s="29" t="s">
-        <v>409</v>
-      </c>
-      <c r="F50" s="43" t="s">
-        <v>411</v>
-      </c>
+      <c r="E50" s="29"/>
+      <c r="F50" s="43"/>
     </row>
     <row r="51" spans="5:6">
-      <c r="E51" s="29" t="s">
-        <v>410</v>
-      </c>
-      <c r="F51" s="52" t="s">
-        <v>412</v>
-      </c>
+      <c r="E51" s="29"/>
+      <c r="F51" s="52"/>
     </row>
     <row r="52" spans="5:6">
-      <c r="E52" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="F52" s="52" t="s">
-        <v>412</v>
-      </c>
+      <c r="E52" s="29"/>
+      <c r="F52" s="52"/>
     </row>
     <row r="53" spans="5:6">
-      <c r="E53" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="F53" s="52" t="s">
-        <v>612</v>
-      </c>
+      <c r="E53" s="29"/>
+      <c r="F53" s="52"/>
     </row>
     <row r="54" spans="5:6">
-      <c r="E54" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="F54" s="52" t="s">
-        <v>613</v>
-      </c>
+      <c r="E54" s="29"/>
+      <c r="F54" s="52"/>
     </row>
     <row r="55" spans="5:6">
-      <c r="E55" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="F55" s="52" t="s">
-        <v>614</v>
-      </c>
+      <c r="E55" s="29"/>
+      <c r="F55" s="52"/>
     </row>
     <row r="56" spans="5:6">
-      <c r="E56" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="F56" s="52" t="s">
-        <v>615</v>
-      </c>
+      <c r="E56" s="29"/>
+      <c r="F56" s="52"/>
     </row>
     <row r="57" spans="5:6">
-      <c r="E57" s="29" t="s">
-        <v>345</v>
-      </c>
-      <c r="F57" s="52" t="s">
-        <v>616</v>
-      </c>
+      <c r="E57" s="29"/>
+      <c r="F57" s="52"/>
     </row>
     <row r="58" spans="5:6">
-      <c r="E58" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="F58" s="52" t="s">
-        <v>617</v>
-      </c>
+      <c r="E58" s="29"/>
+      <c r="F58" s="52"/>
     </row>
     <row r="59" spans="5:6">
-      <c r="E59" s="29" t="s">
-        <v>326</v>
-      </c>
-      <c r="F59" s="52" t="s">
-        <v>619</v>
-      </c>
+      <c r="E59" s="29"/>
+      <c r="F59" s="52"/>
     </row>
     <row r="60" spans="5:6">
-      <c r="E60" s="29" t="s">
-        <v>328</v>
-      </c>
-      <c r="F60" s="52" t="s">
-        <v>619</v>
-      </c>
+      <c r="E60" s="29"/>
+      <c r="F60" s="52"/>
     </row>
     <row r="61" spans="5:6">
-      <c r="E61" s="29" t="s">
-        <v>327</v>
-      </c>
-      <c r="F61" s="34" t="s">
-        <v>618</v>
-      </c>
+      <c r="E61" s="29"/>
+      <c r="F61" s="34"/>
     </row>
     <row r="62" spans="5:6">
-      <c r="E62" s="29" t="s">
-        <v>303</v>
-      </c>
-      <c r="F62" s="52" t="s">
-        <v>620</v>
-      </c>
+      <c r="E62" s="29"/>
+      <c r="F62" s="52"/>
     </row>
     <row r="63" spans="5:6">
-      <c r="E63" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="F63" s="52" t="s">
-        <v>621</v>
-      </c>
+      <c r="E63" s="29"/>
+      <c r="F63" s="52"/>
     </row>
     <row r="64" spans="5:6">
-      <c r="E64" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="F64" s="52" t="s">
-        <v>610</v>
-      </c>
+      <c r="E64" s="29"/>
+      <c r="F64" s="52"/>
     </row>
     <row r="65" spans="5:6">
-      <c r="E65" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="F65" s="52" t="s">
-        <v>611</v>
-      </c>
+      <c r="E65" s="29"/>
+      <c r="F65" s="52"/>
     </row>
     <row r="66" spans="5:6">
-      <c r="E66" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="F66" s="52" t="s">
-        <v>625</v>
-      </c>
+      <c r="E66" s="29"/>
+      <c r="F66" s="52"/>
     </row>
     <row r="67" spans="5:6">
-      <c r="E67" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="F67" s="34" t="s">
-        <v>626</v>
-      </c>
+      <c r="E67" s="29"/>
+      <c r="F67" s="34"/>
     </row>
     <row r="68" spans="5:6">
-      <c r="E68" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="F68" s="52" t="s">
-        <v>627</v>
-      </c>
+      <c r="E68" s="29"/>
+      <c r="F68" s="52"/>
     </row>
     <row r="69" spans="5:6">
-      <c r="E69" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="F69" s="52" t="s">
-        <v>628</v>
-      </c>
+      <c r="E69" s="29"/>
+      <c r="F69" s="52"/>
     </row>
     <row r="70" spans="5:6">
-      <c r="E70" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="F70" s="52" t="s">
-        <v>629</v>
-      </c>
+      <c r="E70" s="29"/>
+      <c r="F70" s="52"/>
     </row>
     <row r="71" spans="5:6">
-      <c r="E71" s="29" t="s">
-        <v>114</v>
-      </c>
+      <c r="E71" s="29"/>
       <c r="F71" s="52"/>
     </row>
     <row r="72" spans="5:6">
-      <c r="E72" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F72" s="34" t="s">
-        <v>630</v>
-      </c>
+      <c r="E72" s="29"/>
+      <c r="F72" s="34"/>
     </row>
     <row r="73" spans="5:6">
-      <c r="E73" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="F73" s="52" t="s">
-        <v>631</v>
-      </c>
+      <c r="E73" s="29"/>
+      <c r="F73" s="52"/>
     </row>
     <row r="74" spans="5:6">
-      <c r="E74" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="F74" s="34" t="s">
-        <v>632</v>
-      </c>
+      <c r="E74" s="29"/>
+      <c r="F74" s="34"/>
     </row>
     <row r="75" spans="5:6">
-      <c r="E75" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="F75" s="34" t="s">
-        <v>633</v>
-      </c>
+      <c r="E75" s="29"/>
+      <c r="F75" s="34"/>
     </row>
     <row r="76" spans="5:6">
-      <c r="E76" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="F76" s="52" t="s">
-        <v>634</v>
-      </c>
+      <c r="E76" s="29"/>
+      <c r="F76" s="52"/>
     </row>
     <row r="77" spans="5:6">
-      <c r="E77" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="F77" s="52" t="s">
-        <v>635</v>
-      </c>
+      <c r="E77" s="29"/>
+      <c r="F77" s="52"/>
     </row>
     <row r="78" spans="5:6">
-      <c r="E78" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="F78" s="34" t="s">
-        <v>420</v>
-      </c>
+      <c r="E78" s="29"/>
+      <c r="F78" s="34"/>
     </row>
     <row r="79" spans="5:6">
-      <c r="E79" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="F79" s="52" t="s">
-        <v>421</v>
-      </c>
+      <c r="E79" s="29"/>
+      <c r="F79" s="52"/>
     </row>
     <row r="80" spans="5:6">
-      <c r="E80" s="29" t="s">
-        <v>135</v>
-      </c>
+      <c r="E80" s="29"/>
       <c r="F80" s="52"/>
     </row>
     <row r="81" spans="5:6">
-      <c r="E81" s="29" t="s">
-        <v>348</v>
-      </c>
-      <c r="F81" s="34" t="s">
-        <v>660</v>
-      </c>
+      <c r="E81" s="29"/>
+      <c r="F81" s="34"/>
     </row>
     <row r="82" spans="5:6">
-      <c r="E82" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="F82" s="34" t="s">
-        <v>661</v>
-      </c>
+      <c r="E82" s="29"/>
+      <c r="F82" s="34"/>
     </row>
     <row r="83" spans="5:6">
-      <c r="E83" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="F83" s="52" t="s">
-        <v>422</v>
-      </c>
+      <c r="E83" s="29"/>
+      <c r="F83" s="52"/>
     </row>
     <row r="84" spans="5:6">
-      <c r="E84" s="29" t="s">
-        <v>346</v>
-      </c>
-      <c r="F84" s="34" t="s">
-        <v>662</v>
-      </c>
+      <c r="E84" s="29"/>
+      <c r="F84" s="34"/>
     </row>
     <row r="85" spans="5:6">
-      <c r="E85" s="29" t="s">
-        <v>347</v>
-      </c>
-      <c r="F85" s="34" t="s">
-        <v>423</v>
-      </c>
+      <c r="E85" s="29"/>
+      <c r="F85" s="34"/>
     </row>
     <row r="86" spans="5:6">
-      <c r="E86" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="F86" s="34" t="s">
-        <v>663</v>
-      </c>
+      <c r="E86" s="29"/>
+      <c r="F86" s="34"/>
     </row>
     <row r="87" spans="5:6">
-      <c r="E87" s="29" t="s">
-        <v>302</v>
-      </c>
-      <c r="F87" s="34" t="s">
-        <v>424</v>
-      </c>
+      <c r="E87" s="29"/>
+      <c r="F87" s="34"/>
     </row>
     <row r="88" spans="5:6">
-      <c r="E88" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="F88" s="34" t="s">
-        <v>425</v>
-      </c>
+      <c r="E88" s="29"/>
+      <c r="F88" s="34"/>
     </row>
     <row r="89" spans="5:6">
-      <c r="E89" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="F89" s="52" t="s">
-        <v>427</v>
-      </c>
+      <c r="E89" s="29"/>
+      <c r="F89" s="52"/>
     </row>
     <row r="90" spans="5:6">
-      <c r="E90" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="F90" s="52" t="s">
-        <v>426</v>
-      </c>
+      <c r="E90" s="29"/>
+      <c r="F90" s="52"/>
     </row>
     <row r="91" spans="5:6">
-      <c r="E91" s="29" t="s">
-        <v>329</v>
-      </c>
-      <c r="F91" s="34" t="s">
-        <v>609</v>
-      </c>
+      <c r="E91" s="29"/>
+      <c r="F91" s="34"/>
     </row>
     <row r="92" spans="5:6">
-      <c r="E92" s="29" t="s">
-        <v>330</v>
-      </c>
-      <c r="F92" s="34" t="s">
-        <v>608</v>
-      </c>
+      <c r="E92" s="29"/>
+      <c r="F92" s="34"/>
     </row>
     <row r="93" spans="5:6">
-      <c r="E93" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="F93" s="52" t="s">
-        <v>664</v>
-      </c>
+      <c r="E93" s="29"/>
+      <c r="F93" s="52"/>
     </row>
     <row r="94" spans="5:6">
-      <c r="E94" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="F94" s="52" t="s">
-        <v>665</v>
-      </c>
+      <c r="E94" s="29"/>
+      <c r="F94" s="52"/>
     </row>
     <row r="95" spans="5:6">
-      <c r="E95" s="29" t="s">
-        <v>164</v>
-      </c>
-      <c r="F95" s="52" t="s">
-        <v>667</v>
-      </c>
+      <c r="E95" s="29"/>
+      <c r="F95" s="52"/>
     </row>
     <row r="96" spans="5:6">
-      <c r="E96" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="F96" s="52" t="s">
-        <v>666</v>
-      </c>
+      <c r="E96" s="29"/>
+      <c r="F96" s="52"/>
     </row>
     <row r="97" spans="5:6">
-      <c r="E97" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="F97" s="52" t="s">
-        <v>668</v>
-      </c>
+      <c r="E97" s="29"/>
+      <c r="F97" s="52"/>
     </row>
     <row r="98" spans="5:6">
-      <c r="E98" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="F98" s="52" t="s">
-        <v>669</v>
-      </c>
+      <c r="E98" s="29"/>
+      <c r="F98" s="52"/>
     </row>
     <row r="99" spans="5:6">
-      <c r="E99" s="29" t="s">
-        <v>171</v>
-      </c>
+      <c r="E99" s="29"/>
       <c r="F99" s="52"/>
     </row>
     <row r="100" spans="5:6">
-      <c r="E100" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="F100" s="52" t="s">
-        <v>670</v>
-      </c>
+      <c r="E100" s="29"/>
+      <c r="F100" s="52"/>
     </row>
     <row r="101" spans="5:6">
-      <c r="E101" s="29" t="s">
-        <v>176</v>
-      </c>
-      <c r="F101" s="52" t="s">
-        <v>554</v>
-      </c>
+      <c r="E101" s="29"/>
+      <c r="F101" s="52"/>
     </row>
     <row r="102" spans="5:6">
-      <c r="E102" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="F102" s="52" t="s">
-        <v>672</v>
-      </c>
+      <c r="E102" s="29"/>
+      <c r="F102" s="52"/>
     </row>
     <row r="103" spans="5:6">
-      <c r="E103" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="F103" s="52" t="s">
-        <v>671</v>
-      </c>
+      <c r="E103" s="29"/>
+      <c r="F103" s="52"/>
     </row>
     <row r="104" spans="5:6">
-      <c r="E104" s="29" t="s">
-        <v>332</v>
-      </c>
-      <c r="F104" s="52" t="s">
-        <v>638</v>
-      </c>
+      <c r="E104" s="29"/>
+      <c r="F104" s="52"/>
     </row>
     <row r="105" spans="5:6">
-      <c r="E105" s="29" t="s">
-        <v>333</v>
-      </c>
-      <c r="F105" s="52" t="s">
-        <v>414</v>
-      </c>
+      <c r="E105" s="29"/>
+      <c r="F105" s="52"/>
     </row>
     <row r="106" spans="5:6">
-      <c r="E106" s="29" t="s">
-        <v>331</v>
-      </c>
-      <c r="F106" s="52" t="s">
-        <v>637</v>
-      </c>
+      <c r="E106" s="29"/>
+      <c r="F106" s="52"/>
     </row>
     <row r="107" spans="5:6">
-      <c r="E107" s="29" t="s">
-        <v>188</v>
-      </c>
-      <c r="F107" s="52" t="s">
-        <v>636</v>
-      </c>
+      <c r="E107" s="29"/>
+      <c r="F107" s="52"/>
     </row>
     <row r="108" spans="5:6">
-      <c r="E108" s="29" t="s">
-        <v>190</v>
-      </c>
-      <c r="F108" s="52" t="s">
-        <v>673</v>
-      </c>
+      <c r="E108" s="29"/>
+      <c r="F108" s="52"/>
     </row>
     <row r="109" spans="5:6">
-      <c r="E109" s="29" t="s">
-        <v>192</v>
-      </c>
-      <c r="F109" s="52" t="s">
-        <v>674</v>
-      </c>
+      <c r="E109" s="29"/>
+      <c r="F109" s="52"/>
     </row>
     <row r="110" spans="5:6">
-      <c r="E110" s="29" t="s">
-        <v>193</v>
-      </c>
+      <c r="E110" s="29"/>
       <c r="F110" s="52"/>
     </row>
     <row r="111" spans="5:6">
-      <c r="E111" s="29" t="s">
-        <v>195</v>
-      </c>
+      <c r="E111" s="29"/>
       <c r="F111" s="34"/>
     </row>
     <row r="112" spans="5:6">
-      <c r="E112" s="29" t="s">
-        <v>334</v>
-      </c>
-      <c r="F112" s="34" t="s">
-        <v>679</v>
-      </c>
+      <c r="E112" s="29"/>
+      <c r="F112" s="34"/>
     </row>
     <row r="113" spans="5:6">
-      <c r="E113" s="29" t="s">
-        <v>199</v>
-      </c>
+      <c r="E113" s="29"/>
       <c r="F113" s="34"/>
     </row>
     <row r="114" spans="5:6">
-      <c r="E114" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="F114" s="52" t="s">
-        <v>680</v>
-      </c>
+      <c r="E114" s="29"/>
+      <c r="F114" s="52"/>
     </row>
     <row r="115" spans="5:6">
-      <c r="E115" s="29" t="s">
-        <v>681</v>
-      </c>
-      <c r="F115" s="34" t="s">
-        <v>683</v>
-      </c>
+      <c r="E115" s="29"/>
+      <c r="F115" s="34"/>
     </row>
     <row r="116" spans="5:6">
-      <c r="E116" s="29" t="s">
-        <v>682</v>
-      </c>
-      <c r="F116" s="34" t="s">
-        <v>684</v>
-      </c>
+      <c r="E116" s="29"/>
+      <c r="F116" s="34"/>
     </row>
     <row r="117" spans="5:6">
-      <c r="E117" s="29" t="s">
-        <v>205</v>
-      </c>
+      <c r="E117" s="29"/>
       <c r="F117" s="52"/>
     </row>
     <row r="118" spans="5:6">
-      <c r="E118" s="29" t="s">
-        <v>336</v>
-      </c>
-      <c r="F118" s="34" t="s">
-        <v>675</v>
-      </c>
+      <c r="E118" s="29"/>
+      <c r="F118" s="34"/>
     </row>
     <row r="119" spans="5:6">
-      <c r="E119" s="29" t="s">
-        <v>337</v>
-      </c>
-      <c r="F119" s="34" t="s">
-        <v>677</v>
-      </c>
+      <c r="E119" s="29"/>
+      <c r="F119" s="34"/>
     </row>
     <row r="120" spans="5:6">
-      <c r="E120" s="29" t="s">
-        <v>338</v>
-      </c>
-      <c r="F120" s="34" t="s">
-        <v>676</v>
-      </c>
+      <c r="E120" s="29"/>
+      <c r="F120" s="34"/>
     </row>
     <row r="121" spans="5:6">
-      <c r="E121" s="29" t="s">
-        <v>339</v>
-      </c>
-      <c r="F121" s="52" t="s">
-        <v>678</v>
-      </c>
+      <c r="E121" s="29"/>
+      <c r="F121" s="52"/>
     </row>
     <row r="122" spans="5:6">
-      <c r="E122" s="29" t="s">
-        <v>211</v>
-      </c>
+      <c r="E122" s="29"/>
       <c r="F122" s="52"/>
     </row>
     <row r="123" spans="5:6">
-      <c r="E123" s="29" t="s">
-        <v>213</v>
-      </c>
-      <c r="F123" s="52" t="s">
-        <v>657</v>
-      </c>
+      <c r="E123" s="29"/>
+      <c r="F123" s="52"/>
     </row>
     <row r="124" spans="5:6">
-      <c r="E124" s="29" t="s">
-        <v>340</v>
-      </c>
-      <c r="F124" s="34" t="s">
-        <v>640</v>
-      </c>
+      <c r="E124" s="29"/>
+      <c r="F124" s="34"/>
     </row>
     <row r="125" spans="5:6">
-      <c r="E125" s="29" t="s">
-        <v>341</v>
-      </c>
-      <c r="F125" s="34" t="s">
-        <v>639</v>
-      </c>
+      <c r="E125" s="29"/>
+      <c r="F125" s="34"/>
     </row>
     <row r="126" spans="5:6">
-      <c r="E126" s="29" t="s">
-        <v>217</v>
-      </c>
-      <c r="F126" s="52" t="s">
-        <v>641</v>
-      </c>
+      <c r="E126" s="29"/>
+      <c r="F126" s="52"/>
     </row>
     <row r="127" spans="5:6">
-      <c r="E127" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="F127" s="52" t="s">
-        <v>656</v>
-      </c>
+      <c r="E127" s="29"/>
+      <c r="F127" s="52"/>
     </row>
     <row r="128" spans="5:6">
-      <c r="E128" s="29" t="s">
-        <v>221</v>
-      </c>
-      <c r="F128" s="52" t="s">
-        <v>655</v>
-      </c>
+      <c r="E128" s="29"/>
+      <c r="F128" s="52"/>
     </row>
     <row r="129" spans="5:6">
-      <c r="E129" s="29" t="s">
-        <v>224</v>
-      </c>
-      <c r="F129" s="52" t="s">
-        <v>643</v>
-      </c>
+      <c r="E129" s="29"/>
+      <c r="F129" s="52"/>
     </row>
     <row r="130" spans="5:6">
-      <c r="E130" s="32" t="s">
-        <v>226</v>
-      </c>
-      <c r="F130" s="34" t="s">
-        <v>642</v>
-      </c>
+      <c r="E130" s="32"/>
+      <c r="F130" s="34"/>
     </row>
     <row r="131" spans="5:6">
-      <c r="E131" s="32" t="s">
-        <v>228</v>
-      </c>
-      <c r="F131" s="34" t="s">
-        <v>644</v>
-      </c>
+      <c r="E131" s="32"/>
+      <c r="F131" s="34"/>
     </row>
     <row r="132" spans="5:6">
-      <c r="E132" s="29" t="s">
-        <v>230</v>
-      </c>
-      <c r="F132" s="52" t="s">
-        <v>645</v>
-      </c>
+      <c r="E132" s="29"/>
+      <c r="F132" s="52"/>
     </row>
     <row r="133" spans="5:6">
-      <c r="E133" s="29" t="s">
-        <v>233</v>
-      </c>
-      <c r="F133" s="34" t="s">
-        <v>654</v>
-      </c>
+      <c r="E133" s="29"/>
+      <c r="F133" s="34"/>
     </row>
     <row r="134" spans="5:6">
-      <c r="E134" s="29" t="s">
-        <v>236</v>
-      </c>
-      <c r="F134" s="52" t="s">
-        <v>653</v>
-      </c>
+      <c r="E134" s="29"/>
+      <c r="F134" s="52"/>
     </row>
     <row r="135" spans="5:6">
-      <c r="E135" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="F135" s="52" t="s">
-        <v>652</v>
-      </c>
+      <c r="E135" s="29"/>
+      <c r="F135" s="52"/>
     </row>
     <row r="136" spans="5:6">
-      <c r="E136" s="29" t="s">
-        <v>240</v>
-      </c>
-      <c r="F136" s="34" t="s">
-        <v>651</v>
-      </c>
+      <c r="E136" s="29"/>
+      <c r="F136" s="34"/>
     </row>
     <row r="137" spans="5:6">
-      <c r="E137" s="29" t="s">
-        <v>243</v>
-      </c>
-      <c r="F137" s="52" t="s">
-        <v>650</v>
-      </c>
+      <c r="E137" s="29"/>
+      <c r="F137" s="52"/>
     </row>
     <row r="138" spans="5:6">
-      <c r="E138" s="29" t="s">
-        <v>244</v>
-      </c>
+      <c r="E138" s="29"/>
       <c r="F138" s="52"/>
     </row>
     <row r="139" spans="5:6">
-      <c r="E139" s="48" t="s">
-        <v>246</v>
-      </c>
-      <c r="F139" s="34" t="s">
-        <v>649</v>
-      </c>
+      <c r="E139" s="48"/>
+      <c r="F139" s="34"/>
     </row>
     <row r="140" spans="5:6">
-      <c r="E140" s="29" t="s">
-        <v>248</v>
-      </c>
-      <c r="F140" s="34" t="s">
-        <v>648</v>
-      </c>
+      <c r="E140" s="29"/>
+      <c r="F140" s="34"/>
     </row>
     <row r="141" spans="5:6">
-      <c r="E141" s="29" t="s">
-        <v>250</v>
-      </c>
-      <c r="F141" s="34" t="s">
-        <v>647</v>
-      </c>
+      <c r="E141" s="29"/>
+      <c r="F141" s="34"/>
     </row>
     <row r="142" spans="5:6">
-      <c r="E142" s="29" t="s">
-        <v>252</v>
-      </c>
-      <c r="F142" s="34" t="s">
-        <v>646</v>
-      </c>
+      <c r="E142" s="29"/>
+      <c r="F142" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -10349,7 +9892,7 @@
         <v>8</v>
       </c>
       <c r="L2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="M2" s="43" t="s">
         <v>555</v>
@@ -10428,7 +9971,7 @@
         <v>9</v>
       </c>
       <c r="L3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="M3" s="43" t="s">
         <v>555</v>
@@ -10506,7 +10049,7 @@
         <v>4</v>
       </c>
       <c r="L4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="M4" s="43" t="s">
         <v>555</v>
@@ -10584,7 +10127,7 @@
         <v>11</v>
       </c>
       <c r="L5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="M5" s="43" t="s">
         <v>555</v>
@@ -10659,7 +10202,7 @@
         <v>4</v>
       </c>
       <c r="L6" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="M6" s="43" t="s">
         <v>555</v>
@@ -10737,7 +10280,7 @@
         <v>3</v>
       </c>
       <c r="L7" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="M7" s="43" t="s">
         <v>555</v>
@@ -10815,7 +10358,7 @@
         <v>7</v>
       </c>
       <c r="L8" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="M8" s="43" t="s">
         <v>555</v>
@@ -10893,7 +10436,7 @@
         <v>7</v>
       </c>
       <c r="L9" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="M9" s="43" t="s">
         <v>555</v>
@@ -10971,7 +10514,7 @@
         <v>6</v>
       </c>
       <c r="L10" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="M10" s="43" t="s">
         <v>555</v>
@@ -11049,7 +10592,7 @@
         <v>3</v>
       </c>
       <c r="L11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="M11" s="43" t="s">
         <v>555</v>
@@ -11127,7 +10670,7 @@
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="M12" s="43" t="s">
         <v>555</v>
@@ -11358,7 +10901,7 @@
         <v>2</v>
       </c>
       <c r="L15" s="52" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="M15" s="43" t="s">
         <v>555</v>
@@ -11514,7 +11057,7 @@
         <v>3</v>
       </c>
       <c r="L17" s="52" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="M17" s="43" t="s">
         <v>555</v>
@@ -11592,7 +11135,7 @@
         <v>2</v>
       </c>
       <c r="L18" s="52" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="M18" s="43" t="s">
         <v>555</v>
@@ -11826,7 +11369,7 @@
         <v>8</v>
       </c>
       <c r="L21" s="54" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="M21" s="43" t="s">
         <v>555</v>
@@ -11904,7 +11447,7 @@
         <v>1</v>
       </c>
       <c r="L22" s="52" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="M22" s="43" t="s">
         <v>555</v>
@@ -11982,7 +11525,7 @@
         <v>1</v>
       </c>
       <c r="L23" s="52" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="M23" s="43" t="s">
         <v>555</v>
@@ -12060,7 +11603,7 @@
         <v>5</v>
       </c>
       <c r="L24" s="52" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="M24" s="43" t="s">
         <v>555</v>
@@ -12450,7 +11993,7 @@
         <v>7</v>
       </c>
       <c r="L29" s="52" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="M29" s="43" t="s">
         <v>555</v>
@@ -12528,7 +12071,7 @@
         <v>1</v>
       </c>
       <c r="L30" s="52" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="M30" s="43" t="s">
         <v>555</v>
@@ -12603,7 +12146,7 @@
         <v>1</v>
       </c>
       <c r="L31" s="52" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="M31" s="43" t="s">
         <v>555</v>
@@ -12681,7 +12224,7 @@
         <v>7</v>
       </c>
       <c r="L32" s="52" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="M32" s="43" t="s">
         <v>555</v>
@@ -12759,7 +12302,7 @@
         <v>1</v>
       </c>
       <c r="L33" s="52" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="M33" s="43" t="s">
         <v>555</v>
@@ -12831,7 +12374,7 @@
         <v>7</v>
       </c>
       <c r="L34" s="52" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="M34" s="43" t="s">
         <v>555</v>
@@ -12909,7 +12452,7 @@
         <v>5</v>
       </c>
       <c r="L35" s="52" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="M35" s="43" t="s">
         <v>555</v>
@@ -12987,7 +12530,7 @@
         <v>5</v>
       </c>
       <c r="L36" s="52" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="M36" s="43" t="s">
         <v>555</v>
@@ -13065,7 +12608,7 @@
         <v>2</v>
       </c>
       <c r="L37" s="34" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="M37" s="43" t="s">
         <v>555</v>
@@ -13143,7 +12686,7 @@
         <v>7</v>
       </c>
       <c r="L38" s="52" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="M38" s="43" t="s">
         <v>555</v>
@@ -13221,7 +12764,7 @@
         <v>1</v>
       </c>
       <c r="L39" s="52" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="M39" s="43" t="s">
         <v>555</v>
@@ -13299,7 +12842,7 @@
         <v>1</v>
       </c>
       <c r="L40" s="52" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="M40" s="43" t="s">
         <v>555</v>
@@ -13377,7 +12920,7 @@
         <v>3</v>
       </c>
       <c r="L41" s="52" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="M41" s="43" t="s">
         <v>555</v>
@@ -13449,7 +12992,7 @@
         <v>4</v>
       </c>
       <c r="L42" s="52" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="M42" s="43" t="s">
         <v>555</v>
@@ -13527,7 +13070,7 @@
         <v>12</v>
       </c>
       <c r="L43" s="34" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="M43" s="43" t="s">
         <v>555</v>
@@ -13605,7 +13148,7 @@
         <v>3</v>
       </c>
       <c r="L44" s="52" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="M44" s="43" t="s">
         <v>555</v>
@@ -13680,7 +13223,7 @@
         <v>1</v>
       </c>
       <c r="L45" s="52" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="M45" s="43" t="s">
         <v>555</v>
@@ -13758,7 +13301,7 @@
         <v>5</v>
       </c>
       <c r="L46" s="52" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="M46" s="43" t="s">
         <v>555</v>
@@ -13912,7 +13455,7 @@
         <v>3</v>
       </c>
       <c r="L48" s="34" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="M48" s="43" t="s">
         <v>555</v>
@@ -13990,7 +13533,7 @@
         <v>18</v>
       </c>
       <c r="L49" s="52" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="M49" s="43" t="s">
         <v>555</v>
@@ -14068,7 +13611,7 @@
         <v>6</v>
       </c>
       <c r="L50" s="34" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="M50" s="43" t="s">
         <v>555</v>
@@ -14146,7 +13689,7 @@
         <v>9</v>
       </c>
       <c r="L51" s="34" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="M51" s="43" t="s">
         <v>555</v>
@@ -14224,7 +13767,7 @@
         <v>4</v>
       </c>
       <c r="L52" s="52" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="M52" s="43" t="s">
         <v>555</v>
@@ -14302,7 +13845,7 @@
         <v>7</v>
       </c>
       <c r="L53" s="52" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="M53" s="43" t="s">
         <v>555</v>
@@ -14612,7 +14155,7 @@
         <v>15</v>
       </c>
       <c r="L57" s="34" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="M57" s="43" t="s">
         <v>555</v>
@@ -14690,7 +14233,7 @@
         <v>3</v>
       </c>
       <c r="L58" s="34" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="M58" s="43" t="s">
         <v>555</v>
@@ -14846,7 +14389,7 @@
         <v>1</v>
       </c>
       <c r="L60" s="34" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="M60" s="43" t="s">
         <v>555</v>
@@ -15002,7 +14545,7 @@
         <v>5</v>
       </c>
       <c r="L62" s="34" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="M62" s="43" t="s">
         <v>555</v>
@@ -15384,7 +14927,7 @@
         <v>2</v>
       </c>
       <c r="L67" s="34" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="M67" s="43" t="s">
         <v>555</v>
@@ -15460,7 +15003,7 @@
         <v>4</v>
       </c>
       <c r="L68" s="34" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="M68" s="43" t="s">
         <v>555</v>
@@ -15535,7 +15078,7 @@
         <v>2</v>
       </c>
       <c r="L69" s="52" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="M69" s="43" t="s">
         <v>555</v>
@@ -15613,7 +15156,7 @@
         <v>2</v>
       </c>
       <c r="L70" s="52" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="M70" s="43" t="s">
         <v>555</v>
@@ -15689,7 +15232,7 @@
         <v>20</v>
       </c>
       <c r="L71" s="52" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="M71" s="43" t="s">
         <v>555</v>
@@ -15767,7 +15310,7 @@
         <v>6</v>
       </c>
       <c r="L72" s="52" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="M72" s="43" t="s">
         <v>555</v>
@@ -15840,7 +15383,7 @@
         <v>1</v>
       </c>
       <c r="L73" s="52" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="M73" s="43" t="s">
         <v>555</v>
@@ -15915,7 +15458,7 @@
         <v>3</v>
       </c>
       <c r="L74" s="52" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="M74" s="43" t="s">
         <v>555</v>
@@ -16060,7 +15603,7 @@
         <v>13</v>
       </c>
       <c r="L76" s="52" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="M76" s="43" t="s">
         <v>555</v>
@@ -16216,7 +15759,7 @@
         <v>2</v>
       </c>
       <c r="L78" s="52" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="M78" s="43" t="s">
         <v>555</v>
@@ -16294,7 +15837,7 @@
         <v>2</v>
       </c>
       <c r="L79" s="52" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="M79" s="43" t="s">
         <v>555</v>
@@ -16372,7 +15915,7 @@
         <v>6</v>
       </c>
       <c r="L80" s="52" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="M80" s="43" t="s">
         <v>555</v>
@@ -16528,7 +16071,7 @@
         <v>6</v>
       </c>
       <c r="L82" s="52" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="M82" s="43" t="s">
         <v>555</v>
@@ -16606,7 +16149,7 @@
         <v>1</v>
       </c>
       <c r="L83" s="52" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="M83" s="43" t="s">
         <v>555</v>
@@ -16682,7 +16225,7 @@
         <v>4</v>
       </c>
       <c r="L84" s="52" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="M84" s="43" t="s">
         <v>555</v>
@@ -16758,7 +16301,7 @@
         <v>6</v>
       </c>
       <c r="L85" s="52" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="M85" s="43" t="s">
         <v>555</v>
@@ -16983,7 +16526,7 @@
         <v>4</v>
       </c>
       <c r="L88" s="34" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="M88" s="43" t="s">
         <v>555</v>
@@ -17133,7 +16676,7 @@
         <v>6</v>
       </c>
       <c r="L90" s="52" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="M90" s="43" t="s">
         <v>555</v>
@@ -17209,7 +16752,7 @@
         <v>4</v>
       </c>
       <c r="L91" s="34" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="M91" s="43" t="s">
         <v>555</v>
@@ -17282,7 +16825,7 @@
         <v>19</v>
       </c>
       <c r="L92" s="34" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="M92" s="43" t="s">
         <v>555</v>
@@ -17436,7 +16979,7 @@
         <v>1</v>
       </c>
       <c r="L94" s="34" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="M94" s="43" t="s">
         <v>555</v>
@@ -17514,7 +17057,7 @@
         <v>8</v>
       </c>
       <c r="L95" s="34" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="M95" s="43" t="s">
         <v>555</v>
@@ -17590,7 +17133,7 @@
         <v>5</v>
       </c>
       <c r="L96" s="34" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="M96" s="43" t="s">
         <v>555</v>
@@ -17665,7 +17208,7 @@
         <v>3</v>
       </c>
       <c r="L97" s="52" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="M97" s="43" t="s">
         <v>555</v>
@@ -17817,7 +17360,7 @@
         <v>14</v>
       </c>
       <c r="L99" s="52" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="M99" s="43" t="s">
         <v>555</v>
@@ -17893,7 +17436,7 @@
         <v>5</v>
       </c>
       <c r="L100" s="34" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="M100" s="43" t="s">
         <v>555</v>
@@ -17969,7 +17512,7 @@
         <v>2</v>
       </c>
       <c r="L101" s="34" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="M101" s="43" t="s">
         <v>555</v>
@@ -18047,7 +17590,7 @@
         <v>1</v>
       </c>
       <c r="L102" s="52" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="M102" s="43" t="s">
         <v>555</v>
@@ -18123,7 +17666,7 @@
         <v>9</v>
       </c>
       <c r="L103" s="52" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="M103" s="43" t="s">
         <v>555</v>
@@ -18198,7 +17741,7 @@
         <v>1</v>
       </c>
       <c r="L104" s="52" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="M104" s="43" t="s">
         <v>555</v>
@@ -18274,7 +17817,7 @@
         <v>9</v>
       </c>
       <c r="L105" s="52" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="M105" s="43" t="s">
         <v>555</v>
@@ -18352,7 +17895,7 @@
         <v>17</v>
       </c>
       <c r="L106" s="34" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="M106" s="43" t="s">
         <v>555</v>
@@ -18428,7 +17971,7 @@
         <v>1</v>
       </c>
       <c r="L107" s="34" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="M107" s="43" t="s">
         <v>555</v>
@@ -18503,7 +18046,7 @@
         <v>9</v>
       </c>
       <c r="L108" s="52" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="M108" s="43" t="s">
         <v>555</v>
@@ -18578,7 +18121,7 @@
         <v>2</v>
       </c>
       <c r="L109" s="34" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="M109" s="43" t="s">
         <v>555</v>
@@ -18656,7 +18199,7 @@
         <v>4</v>
       </c>
       <c r="L110" s="52" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="M110" s="43" t="s">
         <v>555</v>
@@ -18728,7 +18271,7 @@
         <v>9</v>
       </c>
       <c r="L111" s="52" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="M111" s="43" t="s">
         <v>555</v>
@@ -18806,7 +18349,7 @@
         <v>9</v>
       </c>
       <c r="L112" s="34" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="M112" s="43" t="s">
         <v>555</v>
@@ -18878,7 +18421,7 @@
         <v>9</v>
       </c>
       <c r="L113" s="52" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="M113" s="43" t="s">
         <v>555</v>
@@ -19032,7 +18575,7 @@
         <v>2</v>
       </c>
       <c r="L115" s="34" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="M115" s="43" t="s">
         <v>555</v>
@@ -19107,7 +18650,7 @@
         <v>1</v>
       </c>
       <c r="L116" s="34" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="M116" s="43" t="s">
         <v>555</v>
@@ -19182,7 +18725,7 @@
         <v>1</v>
       </c>
       <c r="L117" s="34" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="M117" s="43" t="s">
         <v>555</v>
@@ -19260,7 +18803,7 @@
         <v>1</v>
       </c>
       <c r="L118" s="34" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="M118" s="43" t="s">
         <v>555</v>
@@ -19796,8 +19339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="M60:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="M58" sqref="M58"/>
+    <sheetView topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="M66" sqref="M66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
logout moved to navbar
</commit_message>
<xml_diff>
--- a/markdown + erd + wireframes + spreadsheet/neat-150730.xlsx
+++ b/markdown + erd + wireframes + spreadsheet/neat-150730.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="520" windowWidth="23920" windowHeight="14900" tabRatio="936"/>
+    <workbookView xWindow="360" yWindow="520" windowWidth="23920" windowHeight="14900" tabRatio="936"/>
   </bookViews>
   <sheets>
     <sheet name="neat-todo" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3634" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3628" uniqueCount="679">
   <si>
     <t>Date</t>
   </si>
@@ -1757,12 +1757,6 @@
     <t>if I change any of the data in seeds</t>
   </si>
   <si>
-    <t>NAV BAR</t>
-  </si>
-  <si>
-    <t>SHOW WHISKEY PAGE</t>
-  </si>
-  <si>
     <t>link as many images as possible</t>
   </si>
   <si>
@@ -1796,12 +1790,6 @@
     <t>switches to the nav branch</t>
   </si>
   <si>
-    <t>ADD NEW COMMENT TO SHOW PAGE</t>
-  </si>
-  <si>
-    <t>display all whiskey's comments on whiskey show page</t>
-  </si>
-  <si>
     <t>WHISKEY IMAGES</t>
   </si>
   <si>
@@ -1898,15 +1886,6 @@
     <t>https://img.thewhiskyexchange.com/900/bnvcrn1998.jpg</t>
   </si>
   <si>
-    <t>make edit, delete capable</t>
-  </si>
-  <si>
-    <t>LOGIN</t>
-  </si>
-  <si>
-    <t>style form in the middle of the page</t>
-  </si>
-  <si>
     <t>https://img.thewhiskyexchange.com/540/irish_clo3.jpg</t>
   </si>
   <si>
@@ -2006,12 +1985,6 @@
     <t>https://img.thewhiskyexchange.com/900/brbon_wil39.jpg</t>
   </si>
   <si>
-    <t>why is it still blue and underlined, when I've changed in CSS?</t>
-  </si>
-  <si>
-    <t>yellow #F1C232</t>
-  </si>
-  <si>
     <t>https://img.thewhiskyexchange.com/540/gfcob.12yov1.jpg</t>
   </si>
   <si>
@@ -2088,6 +2061,15 @@
   </si>
   <si>
     <t>image resizing</t>
+  </si>
+  <si>
+    <t>LOGOUT</t>
+  </si>
+  <si>
+    <t>place it in navbar?</t>
+  </si>
+  <si>
+    <t>MAKE COMMENTS DELETEABLE</t>
   </si>
 </sst>
 </file>
@@ -4673,76 +4655,83 @@
     <row r="3" spans="1:6">
       <c r="A3" s="21"/>
       <c r="B3" s="22" t="s">
-        <v>574</v>
+        <v>676</v>
       </c>
       <c r="E3" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="F3" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>657</v>
+        <v>677</v>
       </c>
       <c r="E4" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="F4" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" t="s">
-        <v>658</v>
-      </c>
       <c r="E5" t="s">
-        <v>578</v>
+        <v>576</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" s="22" t="s">
+        <v>678</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" s="22"/>
     </row>
-    <row r="9" spans="1:6">
-      <c r="B9" s="22" t="s">
+    <row r="10" spans="1:6">
+      <c r="B10" s="22" t="s">
         <v>575</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" t="s">
-        <v>588</v>
+        <v>579</v>
       </c>
       <c r="E11" t="s">
-        <v>682</v>
+        <v>673</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="B12" s="22" t="s">
-        <v>587</v>
-      </c>
       <c r="E12" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>621</v>
+        <v>674</v>
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="B14" s="22" t="s">
+        <v>580</v>
+      </c>
       <c r="E14" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="22" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" t="s">
-        <v>623</v>
+        <v>675</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="22" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="26" spans="2:5">
@@ -4755,15 +4744,9 @@
       <c r="E28" s="29"/>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="22" t="s">
-        <v>577</v>
-      </c>
       <c r="E29" s="29"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" t="s">
-        <v>581</v>
-      </c>
       <c r="E30" s="29"/>
     </row>
     <row r="31" spans="2:5">
@@ -4772,78 +4755,63 @@
     <row r="32" spans="2:5">
       <c r="E32" s="29"/>
     </row>
-    <row r="33" spans="2:6">
-      <c r="B33" s="22" t="s">
-        <v>582</v>
-      </c>
+    <row r="33" spans="5:6">
       <c r="E33" s="29"/>
     </row>
-    <row r="34" spans="2:6">
-      <c r="B34" t="s">
-        <v>583</v>
-      </c>
+    <row r="34" spans="5:6">
       <c r="E34" s="29"/>
     </row>
-    <row r="35" spans="2:6">
-      <c r="B35" t="s">
-        <v>584</v>
-      </c>
+    <row r="35" spans="5:6">
       <c r="E35" s="29"/>
     </row>
-    <row r="36" spans="2:6">
+    <row r="36" spans="5:6">
       <c r="E36" s="29"/>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="5:6">
       <c r="E37" s="29"/>
       <c r="F37" s="52"/>
     </row>
-    <row r="38" spans="2:6">
-      <c r="B38" s="22" t="s">
-        <v>589</v>
-      </c>
+    <row r="38" spans="5:6">
       <c r="E38" s="29"/>
       <c r="F38" s="52"/>
     </row>
-    <row r="39" spans="2:6">
-      <c r="B39" t="s">
-        <v>576</v>
-      </c>
+    <row r="39" spans="5:6">
       <c r="E39" s="29"/>
       <c r="F39" s="52"/>
     </row>
-    <row r="40" spans="2:6">
+    <row r="40" spans="5:6">
       <c r="E40" s="29"/>
       <c r="F40" s="52"/>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="5:6">
       <c r="E41" s="29"/>
       <c r="F41" s="52"/>
     </row>
-    <row r="42" spans="2:6">
+    <row r="42" spans="5:6">
       <c r="E42" s="29"/>
       <c r="F42" s="52"/>
     </row>
-    <row r="43" spans="2:6">
+    <row r="43" spans="5:6">
       <c r="E43" s="29"/>
       <c r="F43" s="52"/>
     </row>
-    <row r="44" spans="2:6">
+    <row r="44" spans="5:6">
       <c r="E44" s="29"/>
       <c r="F44" s="52"/>
     </row>
-    <row r="45" spans="2:6">
+    <row r="45" spans="5:6">
       <c r="E45" s="48"/>
       <c r="F45" s="54"/>
     </row>
-    <row r="46" spans="2:6">
+    <row r="46" spans="5:6">
       <c r="E46" s="29"/>
       <c r="F46" s="52"/>
     </row>
-    <row r="47" spans="2:6">
+    <row r="47" spans="5:6">
       <c r="E47" s="29"/>
       <c r="F47" s="52"/>
     </row>
-    <row r="48" spans="2:6">
+    <row r="48" spans="5:6">
       <c r="E48" s="29"/>
       <c r="F48" s="52"/>
     </row>
@@ -9892,7 +9860,7 @@
         <v>8</v>
       </c>
       <c r="L2" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="M2" s="43" t="s">
         <v>555</v>
@@ -9971,7 +9939,7 @@
         <v>9</v>
       </c>
       <c r="L3" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="M3" s="43" t="s">
         <v>555</v>
@@ -10049,7 +10017,7 @@
         <v>4</v>
       </c>
       <c r="L4" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="M4" s="43" t="s">
         <v>555</v>
@@ -10127,7 +10095,7 @@
         <v>11</v>
       </c>
       <c r="L5" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="M5" s="43" t="s">
         <v>555</v>
@@ -10202,7 +10170,7 @@
         <v>4</v>
       </c>
       <c r="L6" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="M6" s="43" t="s">
         <v>555</v>
@@ -10280,7 +10248,7 @@
         <v>3</v>
       </c>
       <c r="L7" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="M7" s="43" t="s">
         <v>555</v>
@@ -10358,7 +10326,7 @@
         <v>7</v>
       </c>
       <c r="L8" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="M8" s="43" t="s">
         <v>555</v>
@@ -10436,7 +10404,7 @@
         <v>7</v>
       </c>
       <c r="L9" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="M9" s="43" t="s">
         <v>555</v>
@@ -10514,7 +10482,7 @@
         <v>6</v>
       </c>
       <c r="L10" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="M10" s="43" t="s">
         <v>555</v>
@@ -10592,7 +10560,7 @@
         <v>3</v>
       </c>
       <c r="L11" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="M11" s="43" t="s">
         <v>555</v>
@@ -10670,7 +10638,7 @@
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="M12" s="43" t="s">
         <v>555</v>
@@ -10901,7 +10869,7 @@
         <v>2</v>
       </c>
       <c r="L15" s="52" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="M15" s="43" t="s">
         <v>555</v>
@@ -11057,7 +11025,7 @@
         <v>3</v>
       </c>
       <c r="L17" s="52" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="M17" s="43" t="s">
         <v>555</v>
@@ -11135,7 +11103,7 @@
         <v>2</v>
       </c>
       <c r="L18" s="52" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="M18" s="43" t="s">
         <v>555</v>
@@ -11369,7 +11337,7 @@
         <v>8</v>
       </c>
       <c r="L21" s="54" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="M21" s="43" t="s">
         <v>555</v>
@@ -11447,7 +11415,7 @@
         <v>1</v>
       </c>
       <c r="L22" s="52" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="M22" s="43" t="s">
         <v>555</v>
@@ -11525,7 +11493,7 @@
         <v>1</v>
       </c>
       <c r="L23" s="52" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="M23" s="43" t="s">
         <v>555</v>
@@ -11603,7 +11571,7 @@
         <v>5</v>
       </c>
       <c r="L24" s="52" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="M24" s="43" t="s">
         <v>555</v>
@@ -11993,7 +11961,7 @@
         <v>7</v>
       </c>
       <c r="L29" s="52" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="M29" s="43" t="s">
         <v>555</v>
@@ -12071,7 +12039,7 @@
         <v>1</v>
       </c>
       <c r="L30" s="52" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="M30" s="43" t="s">
         <v>555</v>
@@ -12146,7 +12114,7 @@
         <v>1</v>
       </c>
       <c r="L31" s="52" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="M31" s="43" t="s">
         <v>555</v>
@@ -12224,7 +12192,7 @@
         <v>7</v>
       </c>
       <c r="L32" s="52" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="M32" s="43" t="s">
         <v>555</v>
@@ -12302,7 +12270,7 @@
         <v>1</v>
       </c>
       <c r="L33" s="52" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="M33" s="43" t="s">
         <v>555</v>
@@ -12374,7 +12342,7 @@
         <v>7</v>
       </c>
       <c r="L34" s="52" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="M34" s="43" t="s">
         <v>555</v>
@@ -12452,7 +12420,7 @@
         <v>5</v>
       </c>
       <c r="L35" s="52" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="M35" s="43" t="s">
         <v>555</v>
@@ -12530,7 +12498,7 @@
         <v>5</v>
       </c>
       <c r="L36" s="52" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="M36" s="43" t="s">
         <v>555</v>
@@ -12608,7 +12576,7 @@
         <v>2</v>
       </c>
       <c r="L37" s="34" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="M37" s="43" t="s">
         <v>555</v>
@@ -12686,7 +12654,7 @@
         <v>7</v>
       </c>
       <c r="L38" s="52" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="M38" s="43" t="s">
         <v>555</v>
@@ -12764,7 +12732,7 @@
         <v>1</v>
       </c>
       <c r="L39" s="52" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="M39" s="43" t="s">
         <v>555</v>
@@ -12842,7 +12810,7 @@
         <v>1</v>
       </c>
       <c r="L40" s="52" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="M40" s="43" t="s">
         <v>555</v>
@@ -12920,7 +12888,7 @@
         <v>3</v>
       </c>
       <c r="L41" s="52" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="M41" s="43" t="s">
         <v>555</v>
@@ -12992,7 +12960,7 @@
         <v>4</v>
       </c>
       <c r="L42" s="52" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
       <c r="M42" s="43" t="s">
         <v>555</v>
@@ -13070,7 +13038,7 @@
         <v>12</v>
       </c>
       <c r="L43" s="34" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
       <c r="M43" s="43" t="s">
         <v>555</v>
@@ -13148,7 +13116,7 @@
         <v>3</v>
       </c>
       <c r="L44" s="52" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
       <c r="M44" s="43" t="s">
         <v>555</v>
@@ -13223,7 +13191,7 @@
         <v>1</v>
       </c>
       <c r="L45" s="52" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
       <c r="M45" s="43" t="s">
         <v>555</v>
@@ -13301,7 +13269,7 @@
         <v>5</v>
       </c>
       <c r="L46" s="52" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
       <c r="M46" s="43" t="s">
         <v>555</v>
@@ -13455,7 +13423,7 @@
         <v>3</v>
       </c>
       <c r="L48" s="34" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="M48" s="43" t="s">
         <v>555</v>
@@ -13533,7 +13501,7 @@
         <v>18</v>
       </c>
       <c r="L49" s="52" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
       <c r="M49" s="43" t="s">
         <v>555</v>
@@ -13611,7 +13579,7 @@
         <v>6</v>
       </c>
       <c r="L50" s="34" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="M50" s="43" t="s">
         <v>555</v>
@@ -13689,7 +13657,7 @@
         <v>9</v>
       </c>
       <c r="L51" s="34" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="M51" s="43" t="s">
         <v>555</v>
@@ -13767,7 +13735,7 @@
         <v>4</v>
       </c>
       <c r="L52" s="52" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
       <c r="M52" s="43" t="s">
         <v>555</v>
@@ -13845,7 +13813,7 @@
         <v>7</v>
       </c>
       <c r="L53" s="52" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
       <c r="M53" s="43" t="s">
         <v>555</v>
@@ -14155,7 +14123,7 @@
         <v>15</v>
       </c>
       <c r="L57" s="34" t="s">
-        <v>659</v>
+        <v>650</v>
       </c>
       <c r="M57" s="43" t="s">
         <v>555</v>
@@ -14233,7 +14201,7 @@
         <v>3</v>
       </c>
       <c r="L58" s="34" t="s">
-        <v>660</v>
+        <v>651</v>
       </c>
       <c r="M58" s="43" t="s">
         <v>555</v>
@@ -14389,7 +14357,7 @@
         <v>1</v>
       </c>
       <c r="L60" s="34" t="s">
-        <v>661</v>
+        <v>652</v>
       </c>
       <c r="M60" s="43" t="s">
         <v>555</v>
@@ -14545,7 +14513,7 @@
         <v>5</v>
       </c>
       <c r="L62" s="34" t="s">
-        <v>662</v>
+        <v>653</v>
       </c>
       <c r="M62" s="43" t="s">
         <v>555</v>
@@ -14927,7 +14895,7 @@
         <v>2</v>
       </c>
       <c r="L67" s="34" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="M67" s="43" t="s">
         <v>555</v>
@@ -15003,7 +14971,7 @@
         <v>4</v>
       </c>
       <c r="L68" s="34" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="M68" s="43" t="s">
         <v>555</v>
@@ -15078,7 +15046,7 @@
         <v>2</v>
       </c>
       <c r="L69" s="52" t="s">
-        <v>663</v>
+        <v>654</v>
       </c>
       <c r="M69" s="43" t="s">
         <v>555</v>
@@ -15156,7 +15124,7 @@
         <v>2</v>
       </c>
       <c r="L70" s="52" t="s">
-        <v>664</v>
+        <v>655</v>
       </c>
       <c r="M70" s="43" t="s">
         <v>555</v>
@@ -15232,7 +15200,7 @@
         <v>20</v>
       </c>
       <c r="L71" s="52" t="s">
-        <v>666</v>
+        <v>657</v>
       </c>
       <c r="M71" s="43" t="s">
         <v>555</v>
@@ -15310,7 +15278,7 @@
         <v>6</v>
       </c>
       <c r="L72" s="52" t="s">
-        <v>665</v>
+        <v>656</v>
       </c>
       <c r="M72" s="43" t="s">
         <v>555</v>
@@ -15383,7 +15351,7 @@
         <v>1</v>
       </c>
       <c r="L73" s="52" t="s">
-        <v>667</v>
+        <v>658</v>
       </c>
       <c r="M73" s="43" t="s">
         <v>555</v>
@@ -15458,7 +15426,7 @@
         <v>3</v>
       </c>
       <c r="L74" s="52" t="s">
-        <v>668</v>
+        <v>659</v>
       </c>
       <c r="M74" s="43" t="s">
         <v>555</v>
@@ -15603,7 +15571,7 @@
         <v>13</v>
       </c>
       <c r="L76" s="52" t="s">
-        <v>669</v>
+        <v>660</v>
       </c>
       <c r="M76" s="43" t="s">
         <v>555</v>
@@ -15759,7 +15727,7 @@
         <v>2</v>
       </c>
       <c r="L78" s="52" t="s">
-        <v>671</v>
+        <v>662</v>
       </c>
       <c r="M78" s="43" t="s">
         <v>555</v>
@@ -15837,7 +15805,7 @@
         <v>2</v>
       </c>
       <c r="L79" s="52" t="s">
-        <v>670</v>
+        <v>661</v>
       </c>
       <c r="M79" s="43" t="s">
         <v>555</v>
@@ -15915,7 +15883,7 @@
         <v>6</v>
       </c>
       <c r="L80" s="52" t="s">
-        <v>637</v>
+        <v>630</v>
       </c>
       <c r="M80" s="43" t="s">
         <v>555</v>
@@ -16071,7 +16039,7 @@
         <v>6</v>
       </c>
       <c r="L82" s="52" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
       <c r="M82" s="43" t="s">
         <v>555</v>
@@ -16149,7 +16117,7 @@
         <v>1</v>
       </c>
       <c r="L83" s="52" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
       <c r="M83" s="43" t="s">
         <v>555</v>
@@ -16225,7 +16193,7 @@
         <v>4</v>
       </c>
       <c r="L84" s="52" t="s">
-        <v>672</v>
+        <v>663</v>
       </c>
       <c r="M84" s="43" t="s">
         <v>555</v>
@@ -16301,7 +16269,7 @@
         <v>6</v>
       </c>
       <c r="L85" s="52" t="s">
-        <v>673</v>
+        <v>664</v>
       </c>
       <c r="M85" s="43" t="s">
         <v>555</v>
@@ -16526,7 +16494,7 @@
         <v>4</v>
       </c>
       <c r="L88" s="34" t="s">
-        <v>678</v>
+        <v>669</v>
       </c>
       <c r="M88" s="43" t="s">
         <v>555</v>
@@ -16676,7 +16644,7 @@
         <v>6</v>
       </c>
       <c r="L90" s="52" t="s">
-        <v>679</v>
+        <v>670</v>
       </c>
       <c r="M90" s="43" t="s">
         <v>555</v>
@@ -16752,7 +16720,7 @@
         <v>4</v>
       </c>
       <c r="L91" s="34" t="s">
-        <v>680</v>
+        <v>671</v>
       </c>
       <c r="M91" s="43" t="s">
         <v>555</v>
@@ -16825,7 +16793,7 @@
         <v>19</v>
       </c>
       <c r="L92" s="34" t="s">
-        <v>681</v>
+        <v>672</v>
       </c>
       <c r="M92" s="43" t="s">
         <v>555</v>
@@ -16979,7 +16947,7 @@
         <v>1</v>
       </c>
       <c r="L94" s="34" t="s">
-        <v>674</v>
+        <v>665</v>
       </c>
       <c r="M94" s="43" t="s">
         <v>555</v>
@@ -17057,7 +17025,7 @@
         <v>8</v>
       </c>
       <c r="L95" s="34" t="s">
-        <v>676</v>
+        <v>667</v>
       </c>
       <c r="M95" s="43" t="s">
         <v>555</v>
@@ -17133,7 +17101,7 @@
         <v>5</v>
       </c>
       <c r="L96" s="34" t="s">
-        <v>675</v>
+        <v>666</v>
       </c>
       <c r="M96" s="43" t="s">
         <v>555</v>
@@ -17208,7 +17176,7 @@
         <v>3</v>
       </c>
       <c r="L97" s="52" t="s">
-        <v>677</v>
+        <v>668</v>
       </c>
       <c r="M97" s="43" t="s">
         <v>555</v>
@@ -17360,7 +17328,7 @@
         <v>14</v>
       </c>
       <c r="L99" s="52" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
       <c r="M99" s="43" t="s">
         <v>555</v>
@@ -17436,7 +17404,7 @@
         <v>5</v>
       </c>
       <c r="L100" s="34" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="M100" s="43" t="s">
         <v>555</v>
@@ -17512,7 +17480,7 @@
         <v>2</v>
       </c>
       <c r="L101" s="34" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
       <c r="M101" s="43" t="s">
         <v>555</v>
@@ -17590,7 +17558,7 @@
         <v>1</v>
       </c>
       <c r="L102" s="52" t="s">
-        <v>640</v>
+        <v>633</v>
       </c>
       <c r="M102" s="43" t="s">
         <v>555</v>
@@ -17666,7 +17634,7 @@
         <v>9</v>
       </c>
       <c r="L103" s="52" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="M103" s="43" t="s">
         <v>555</v>
@@ -17741,7 +17709,7 @@
         <v>1</v>
       </c>
       <c r="L104" s="52" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="M104" s="43" t="s">
         <v>555</v>
@@ -17817,7 +17785,7 @@
         <v>9</v>
       </c>
       <c r="L105" s="52" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
       <c r="M105" s="43" t="s">
         <v>555</v>
@@ -17895,7 +17863,7 @@
         <v>17</v>
       </c>
       <c r="L106" s="34" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
       <c r="M106" s="43" t="s">
         <v>555</v>
@@ -17971,7 +17939,7 @@
         <v>1</v>
       </c>
       <c r="L107" s="34" t="s">
-        <v>643</v>
+        <v>636</v>
       </c>
       <c r="M107" s="43" t="s">
         <v>555</v>
@@ -18046,7 +18014,7 @@
         <v>9</v>
       </c>
       <c r="L108" s="52" t="s">
-        <v>644</v>
+        <v>637</v>
       </c>
       <c r="M108" s="43" t="s">
         <v>555</v>
@@ -18121,7 +18089,7 @@
         <v>2</v>
       </c>
       <c r="L109" s="34" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="M109" s="43" t="s">
         <v>555</v>
@@ -18199,7 +18167,7 @@
         <v>4</v>
       </c>
       <c r="L110" s="52" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="M110" s="43" t="s">
         <v>555</v>
@@ -18271,7 +18239,7 @@
         <v>9</v>
       </c>
       <c r="L111" s="52" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="M111" s="43" t="s">
         <v>555</v>
@@ -18349,7 +18317,7 @@
         <v>9</v>
       </c>
       <c r="L112" s="34" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
       <c r="M112" s="43" t="s">
         <v>555</v>
@@ -18421,7 +18389,7 @@
         <v>9</v>
       </c>
       <c r="L113" s="52" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
       <c r="M113" s="43" t="s">
         <v>555</v>
@@ -18575,7 +18543,7 @@
         <v>2</v>
       </c>
       <c r="L115" s="34" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="M115" s="43" t="s">
         <v>555</v>
@@ -18650,7 +18618,7 @@
         <v>1</v>
       </c>
       <c r="L116" s="34" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
       <c r="M116" s="43" t="s">
         <v>555</v>
@@ -18725,7 +18693,7 @@
         <v>1</v>
       </c>
       <c r="L117" s="34" t="s">
-        <v>646</v>
+        <v>639</v>
       </c>
       <c r="M117" s="43" t="s">
         <v>555</v>
@@ -18803,7 +18771,7 @@
         <v>1</v>
       </c>
       <c r="L118" s="34" t="s">
-        <v>645</v>
+        <v>638</v>
       </c>
       <c r="M118" s="43" t="s">
         <v>555</v>

</xml_diff>